<commit_message>
fix: alignment by year
</commit_message>
<xml_diff>
--- a/database/seeders/data/CODE_LinkFunction.xlsx
+++ b/database/seeders/data/CODE_LinkFunction.xlsx
@@ -1,28 +1,203 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JEJE\Documents\GitHub\sig-kondisi-jalaan\database\seeders\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257751F0-10C6-44D4-9AA1-9AD61CEB3847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="CODE_LinkFunction"/>
+    <sheet name="CODE_LinkFunction" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CODE_LinkFunction">'CODE_LinkFunction'!$A$1:$D$7</definedName>
+    <definedName name="CODE_LinkFunction">CODE_LinkFunction!$A$1:$D$7</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>CodeDescription_Eng</t>
+  </si>
+  <si>
+    <t>CodeDescription_Ind</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Arterial</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>Collector 2</t>
+  </si>
+  <si>
+    <t>Kollector 2</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>Collector 3</t>
+  </si>
+  <si>
+    <t>Kollector 3</t>
+  </si>
+  <si>
+    <t>K4</t>
+  </si>
+  <si>
+    <t>Collector 4</t>
+  </si>
+  <si>
+    <t>Kollector 4</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Lokal</t>
+  </si>
+  <si>
+    <t>Ln</t>
+  </si>
+  <si>
+    <t>Neighborhood</t>
+  </si>
+  <si>
+    <t>Lingkungan</t>
+  </si>
+  <si>
+    <t>Jalan Kolektor Primer 1 (JKP-1)</t>
+  </si>
+  <si>
+    <t>Jalan Kolektor Primer 2 (JKP-2)</t>
+  </si>
+  <si>
+    <t>Jalan Kolektor Primer 3 (JKP-3)</t>
+  </si>
+  <si>
+    <t>Jalan Kolektor Primer 4 (JKP-4)</t>
+  </si>
+  <si>
+    <t>Primary Collector Road 1 (JKP-1)</t>
+  </si>
+  <si>
+    <t>Primary Collector Road 2 (JKP-2)</t>
+  </si>
+  <si>
+    <t>Primary Collector Road 3 (JKP-3)</t>
+  </si>
+  <si>
+    <t>Primary Collector Road 4 (JKP-4)</t>
+  </si>
+  <si>
+    <t>JLP</t>
+  </si>
+  <si>
+    <t>Primary Local Road (JLP)</t>
+  </si>
+  <si>
+    <t>Jalan Lokal Primer (JLP)</t>
+  </si>
+  <si>
+    <t>Primary Neighborhood Road (J.Ling.P)</t>
+  </si>
+  <si>
+    <t>Jalan Lingkungan Primer (J.Ling.P)</t>
+  </si>
+  <si>
+    <t>JLS</t>
+  </si>
+  <si>
+    <t>Secondary Local Road (JLS)</t>
+  </si>
+  <si>
+    <t>Jalan Lokal Sekunder (JLS)</t>
+  </si>
+  <si>
+    <t>Secondary Neighborhood Road (J.Ling.S)</t>
+  </si>
+  <si>
+    <t>Jalan Lingkungan Sekunder (J.Ling.S)</t>
+  </si>
+  <si>
+    <t>JAS</t>
+  </si>
+  <si>
+    <t>Jalan Arteri Sekunder (JAS)</t>
+  </si>
+  <si>
+    <t>JKS</t>
+  </si>
+  <si>
+    <t>Secondary Arterial Road (JAS)</t>
+  </si>
+  <si>
+    <t>Secondary Collector Road (JKS)</t>
+  </si>
+  <si>
+    <t>Jalan Kolektor Sekunder (JKS)</t>
+  </si>
+  <si>
+    <t>JKP 1</t>
+  </si>
+  <si>
+    <t>JKP 2</t>
+  </si>
+  <si>
+    <t>JKP 3</t>
+  </si>
+  <si>
+    <t>JKP 4</t>
+  </si>
+  <si>
+    <t>J.Ling.P</t>
+  </si>
+  <si>
+    <t>J.Ling.S</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -55,6 +230,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -101,7 +284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,9 +316,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,6 +368,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,158 +561,259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row outlineLevel="0" r="1">
-      <c r="A1" s="0" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>CodeDescription_Eng</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
-        <is>
-          <t>CodeDescription_Ind</t>
-        </is>
-      </c>
-      <c r="D1" s="0" t="inlineStr">
-        <is>
-          <t>Order</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Arterial</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>Arterial</t>
-        </is>
-      </c>
-      <c r="D2" s="0">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>K2</t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Collector 2</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>Kollector 2</t>
-        </is>
-      </c>
-      <c r="D3" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>K3</t>
-        </is>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>Collector 3</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>Kollector 3</t>
-        </is>
-      </c>
-      <c r="D4" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>K4</t>
-        </is>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>Collector 4</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>Kollector 4</t>
-        </is>
-      </c>
-      <c r="D5" s="0">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>Local</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>Lokal</t>
-        </is>
-      </c>
-      <c r="D6" s="0">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="0" t="inlineStr">
-        <is>
-          <t>Ln</t>
-        </is>
-      </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>Neighborhood</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>Lingkungan</t>
-        </is>
-      </c>
-      <c r="D7" s="0">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>